<commit_message>
Update With Lab PRBS data
</commit_message>
<xml_diff>
--- a/src/systemParameterIdentification/dataLogging.xlsx
+++ b/src/systemParameterIdentification/dataLogging.xlsx
@@ -12,6 +12,8 @@
     <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Log3" sheetId="3" r:id="rId3"/>
     <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Log4" sheetId="4" r:id="rId4"/>
     <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Log5" sheetId="5" r:id="rId5"/>
+    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Log6" sheetId="6" r:id="rId6"/>
+    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Log7" sheetId="7" r:id="rId7"/>
   </s:sheets>
   <s:definedNames/>
   <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -58,6 +60,12 @@
   </si>
   <si>
     <t>Tue Mar 15 23:11:08 2016</t>
+  </si>
+  <si>
+    <t>Wed Mar 16 15:42:23 2016</t>
+  </si>
+  <si>
+    <t>Wed Mar 16 15:49:59 2016</t>
   </si>
 </sst>
 </file>
@@ -10450,6 +10458,741 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" width="9.1" customWidth="1" max="1"/>
+    <col min="2" width="9.1" customWidth="1" max="2"/>
+    <col min="3" width="9.1" customWidth="1" max="3"/>
+    <col min="4" width="9.1" customWidth="1" max="4"/>
+    <col min="5" width="9.1" customWidth="1" max="5"/>
+    <col min="6" width="9.1" customWidth="1" max="6"/>
+    <col min="7" width="9.1" customWidth="1" max="7"/>
+  </cols>
+  <sheetData>
+    <row spans="1:7" r="1">
+      <c t="s" r="A1">
+        <v>3</v>
+      </c>
+      <c t="s" r="B1">
+        <v>12</v>
+      </c>
+    </row>
+    <row spans="1:7" r="3">
+      <c t="s" r="A3">
+        <v>4</v>
+      </c>
+      <c t="s" r="B3">
+        <v>6</v>
+      </c>
+      <c t="s" r="C3">
+        <v>0</v>
+      </c>
+      <c t="s" r="D3">
+        <v>7</v>
+      </c>
+      <c t="s" r="E3">
+        <v>5</v>
+      </c>
+      <c t="s" r="F3">
+        <v>1</v>
+      </c>
+      <c t="s" r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row spans="1:7" r="4">
+      <c t="n" r="A4">
+        <v>0.0009999275207519531</v>
+      </c>
+      <c t="n" r="B4">
+        <v>35.93319928362619</v>
+      </c>
+      <c t="n" r="C4">
+        <v>0</v>
+      </c>
+      <c t="n" r="D4">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E4">
+        <v>40</v>
+      </c>
+      <c t="n" r="F4">
+        <v>0.8726883592757834</v>
+      </c>
+      <c t="n" r="G4">
+        <v>0.14046549089770402</v>
+      </c>
+    </row>
+    <row spans="1:7" r="5">
+      <c t="n" r="A5">
+        <v>40.00099992752075</v>
+      </c>
+      <c t="n" r="B5">
+        <v>39.033975167287515</v>
+      </c>
+      <c t="n" r="C5">
+        <v>0</v>
+      </c>
+      <c t="n" r="D5">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E5">
+        <v>100</v>
+      </c>
+      <c t="n" r="F5">
+        <v>0.7163546569173938</v>
+      </c>
+      <c t="n" r="G5">
+        <v>0.3339207038481812</v>
+      </c>
+    </row>
+    <row spans="1:7" r="6">
+      <c t="n" r="A6">
+        <v>80.0019998550415</v>
+      </c>
+      <c t="n" r="B6">
+        <v>31.03483491698797</v>
+      </c>
+      <c t="n" r="C6">
+        <v>0</v>
+      </c>
+      <c t="n" r="D6">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E6">
+        <v>0</v>
+      </c>
+      <c t="n" r="F6">
+        <v>1.451773241600581</v>
+      </c>
+      <c t="n" r="G6">
+        <v>-0.25601925712454654</v>
+      </c>
+    </row>
+    <row spans="1:7" r="7">
+      <c t="n" r="A7">
+        <v>120.00099992752075</v>
+      </c>
+      <c t="n" r="B7">
+        <v>22.977419850428806</v>
+      </c>
+      <c t="n" r="C7">
+        <v>0</v>
+      </c>
+      <c t="n" r="D7">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E7">
+        <v>0</v>
+      </c>
+      <c t="n" r="F7">
+        <v>0.741891634918841</v>
+      </c>
+      <c t="n" r="G7">
+        <v>0.6298063657286977</v>
+      </c>
+    </row>
+    <row spans="1:7" r="8">
+      <c t="n" r="A8">
+        <v>160.0</v>
+      </c>
+      <c t="n" r="B8">
+        <v>27.706051296647992</v>
+      </c>
+      <c t="n" r="C8">
+        <v>0</v>
+      </c>
+      <c t="n" r="D8">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E8">
+        <v>100</v>
+      </c>
+      <c t="n" r="F8">
+        <v>1.2043497720614438</v>
+      </c>
+      <c t="n" r="G8">
+        <v>0.25884948477102326</v>
+      </c>
+    </row>
+    <row spans="1:7" r="9">
+      <c t="n" r="A9">
+        <v>199.99899983406067</v>
+      </c>
+      <c t="n" r="B9">
+        <v>30.73692414571351</v>
+      </c>
+      <c t="n" r="C9">
+        <v>0</v>
+      </c>
+      <c t="n" r="D9">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E9">
+        <v>100</v>
+      </c>
+      <c t="n" r="F9">
+        <v>1.4992702757300553</v>
+      </c>
+      <c t="n" r="G9">
+        <v>-0.1078971777120829</v>
+      </c>
+    </row>
+    <row spans="1:7" r="10">
+      <c t="n" r="A10">
+        <v>239.99899983406067</v>
+      </c>
+      <c t="n" r="B10">
+        <v>22.946814329570003</v>
+      </c>
+      <c t="n" r="C10">
+        <v>0</v>
+      </c>
+      <c t="n" r="D10">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E10">
+        <v>0</v>
+      </c>
+      <c t="n" r="F10">
+        <v>1.747515042021345</v>
+      </c>
+      <c t="n" r="G10">
+        <v>-0.3075761376625977</v>
+      </c>
+    </row>
+    <row spans="1:7" r="11">
+      <c t="n" r="A11">
+        <v>279.9979999065399</v>
+      </c>
+      <c t="n" r="B11">
+        <v>26.8511666315705</v>
+      </c>
+      <c t="n" r="C11">
+        <v>0</v>
+      </c>
+      <c t="n" r="D11">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E11">
+        <v>100</v>
+      </c>
+      <c t="n" r="F11">
+        <v>1.172391728625611</v>
+      </c>
+      <c t="n" r="G11">
+        <v>0.40805590313024753</v>
+      </c>
+    </row>
+    <row spans="1:7" r="12">
+      <c t="n" r="A12">
+        <v>319.99899983406067</v>
+      </c>
+      <c t="n" r="B12">
+        <v>19.21372652447492</v>
+      </c>
+      <c t="n" r="C12">
+        <v>0</v>
+      </c>
+      <c t="n" r="D12">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E12">
+        <v>0</v>
+      </c>
+      <c t="n" r="F12">
+        <v>2.159355880249014</v>
+      </c>
+      <c t="n" r="G12">
+        <v>-0.387351456146498</v>
+      </c>
+    </row>
+    <row spans="1:7" r="13">
+      <c t="n" r="A13">
+        <v>359.99899983406067</v>
+      </c>
+      <c t="n" r="B13">
+        <v>24.686907023340694</v>
+      </c>
+      <c t="n" r="C13">
+        <v>0</v>
+      </c>
+      <c t="n" r="D13">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E13">
+        <v>100</v>
+      </c>
+      <c t="n" r="F13">
+        <v>1.2896920391939184</v>
+      </c>
+      <c t="n" r="G13">
+        <v>0.6926412478166487</v>
+      </c>
+    </row>
+    <row spans="1:7" r="14">
+      <c t="n" r="A14">
+        <v>399.9979999065399</v>
+      </c>
+      <c t="n" r="B14">
+        <v>16.98029368105073</v>
+      </c>
+      <c t="n" r="C14">
+        <v>0</v>
+      </c>
+      <c t="n" r="D14">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E14">
+        <v>0</v>
+      </c>
+      <c t="n" r="F14">
+        <v>2.787932051650233</v>
+      </c>
+      <c t="n" r="G14">
+        <v>-0.517979795871555</v>
+      </c>
+    </row>
+    <row spans="1:7" r="15">
+      <c t="n" r="A15">
+        <v>439.9979999065399</v>
+      </c>
+      <c t="n" r="B15">
+        <v>11.026008525667306</v>
+      </c>
+      <c t="n" r="C15">
+        <v>0</v>
+      </c>
+      <c t="n" r="D15">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E15">
+        <v>0</v>
+      </c>
+      <c t="n" r="F15">
+        <v>0.6644325322934646</v>
+      </c>
+      <c t="n" r="G15">
+        <v>2.112097229549415</v>
+      </c>
+    </row>
+    <row spans="1:7" r="16">
+      <c t="n" r="A16">
+        <v>479.9979999065399</v>
+      </c>
+      <c t="n" r="B16">
+        <v>6.231911006630713</v>
+      </c>
+      <c t="n" r="C16">
+        <v>0</v>
+      </c>
+      <c t="n" r="D16">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E16">
+        <v>0</v>
+      </c>
+      <c t="n" r="F16">
+        <v>0.5665350337116167</v>
+      </c>
+      <c t="n" r="G16">
+        <v>2.191379567104027</v>
+      </c>
+    </row>
+    <row spans="1:7" r="17">
+      <c t="n" r="A17">
+        <v>519.9979999065399</v>
+      </c>
+      <c t="n" r="B17">
+        <v>13.35249149398372</v>
+      </c>
+      <c t="n" r="C17">
+        <v>0</v>
+      </c>
+      <c t="n" r="D17">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E17">
+        <v>100</v>
+      </c>
+      <c t="n" r="F17">
+        <v>2.0639738616114385</v>
+      </c>
+      <c t="n" r="G17">
+        <v>0.3528783318954183</v>
+      </c>
+    </row>
+    <row spans="1:7" r="18">
+      <c t="n" r="A18">
+        <v>559.9979999065399</v>
+      </c>
+      <c t="n" r="B18">
+        <v>19.057098349076064</v>
+      </c>
+      <c t="n" r="C18">
+        <v>0</v>
+      </c>
+      <c t="n" r="D18">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E18">
+        <v>100</v>
+      </c>
+      <c t="n" r="F18">
+        <v>2.6906336488950298</v>
+      </c>
+      <c t="n" r="G18">
+        <v>-0.16853125826269044</v>
+      </c>
+    </row>
+    <row spans="1:7" r="19">
+      <c t="n" r="A19">
+        <v>599.9969999790192</v>
+      </c>
+      <c t="n" r="B19">
+        <v>13.443004177115851</v>
+      </c>
+      <c t="n" r="C19">
+        <v>0</v>
+      </c>
+      <c t="n" r="D19">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E19">
+        <v>0</v>
+      </c>
+      <c t="n" r="F19">
+        <v>2.898068558396268</v>
+      </c>
+      <c t="n" r="G19">
+        <v>-0.41778593517381774</v>
+      </c>
+    </row>
+    <row spans="1:7" r="20">
+      <c t="n" r="A20">
+        <v>639.9979999065399</v>
+      </c>
+      <c t="n" r="B20">
+        <v>8.147693472612058</v>
+      </c>
+      <c t="n" r="C20">
+        <v>0</v>
+      </c>
+      <c t="n" r="D20">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E20">
+        <v>0</v>
+      </c>
+      <c t="n" r="F20">
+        <v>0.627160620447222</v>
+      </c>
+      <c t="n" r="G20">
+        <v>1.4708368390401685</v>
+      </c>
+    </row>
+    <row spans="1:7" r="21">
+      <c t="n" r="A21">
+        <v>679.9979999065399</v>
+      </c>
+      <c t="n" r="B21">
+        <v>4.029421178810437</v>
+      </c>
+      <c t="n" r="C21">
+        <v>0</v>
+      </c>
+      <c t="n" r="D21">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E21">
+        <v>0</v>
+      </c>
+      <c t="n" r="F21">
+        <v>0.4984489590586714</v>
+      </c>
+      <c t="n" r="G21">
+        <v>1.625075160969069</v>
+      </c>
+    </row>
+    <row spans="1:7" r="22">
+      <c t="n" r="A22">
+        <v>719.9979999065399</v>
+      </c>
+      <c t="n" r="B22">
+        <v>1.1388019894559074</v>
+      </c>
+      <c t="n" r="C22">
+        <v>0</v>
+      </c>
+      <c t="n" r="D22">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E22">
+        <v>0</v>
+      </c>
+      <c t="n" r="F22">
+        <v>0.3029409353122563</v>
+      </c>
+      <c t="n" r="G22">
+        <v>1.7899812102016348</v>
+      </c>
+    </row>
+    <row spans="1:7" r="23">
+      <c t="n" r="A23">
+        <v>759.9969999790192</v>
+      </c>
+      <c t="n" r="B23">
+        <v>10.271096523958475</v>
+      </c>
+      <c t="n" r="C23">
+        <v>0</v>
+      </c>
+      <c t="n" r="D23">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E23">
+        <v>100</v>
+      </c>
+      <c t="n" r="F23">
+        <v>3.767095738777922</v>
+      </c>
+      <c t="n" r="G23">
+        <v>-2.1870212125393547</v>
+      </c>
+    </row>
+    <row spans="1:7" r="24">
+      <c t="n" r="A24">
+        <v>799.9979999065399</v>
+      </c>
+      <c t="n" r="B24">
+        <v>5.610730090849676</v>
+      </c>
+      <c t="n" r="C24">
+        <v>0</v>
+      </c>
+      <c t="n" r="D24">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E24">
+        <v>0</v>
+      </c>
+      <c t="n" r="F24">
+        <v>1.7628509569017332</v>
+      </c>
+      <c t="n" r="G24">
+        <v>-0.12551221072150787</v>
+      </c>
+    </row>
+    <row spans="1:7" r="25">
+      <c t="n" r="A25">
+        <v>839.9979999065399</v>
+      </c>
+      <c t="n" r="B25">
+        <v>2.1973201275748835</v>
+      </c>
+      <c t="n" r="C25">
+        <v>0</v>
+      </c>
+      <c t="n" r="D25">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E25">
+        <v>0</v>
+      </c>
+      <c t="n" r="F25">
+        <v>0.46599514819084353</v>
+      </c>
+      <c t="n" r="G25">
+        <v>1.1352072927234342</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" width="9.1" customWidth="1" max="1"/>
+    <col min="2" width="9.1" customWidth="1" max="2"/>
+    <col min="3" width="9.1" customWidth="1" max="3"/>
+    <col min="4" width="9.1" customWidth="1" max="4"/>
+    <col min="5" width="9.1" customWidth="1" max="5"/>
+    <col min="6" width="9.1" customWidth="1" max="6"/>
+    <col min="7" width="9.1" customWidth="1" max="7"/>
+  </cols>
+  <sheetData>
+    <row spans="1:7" r="1">
+      <c t="s" r="A1">
+        <v>3</v>
+      </c>
+      <c t="s" r="B1">
+        <v>13</v>
+      </c>
+    </row>
+    <row spans="1:7" r="3">
+      <c t="s" r="A3">
+        <v>4</v>
+      </c>
+      <c t="s" r="B3">
+        <v>6</v>
+      </c>
+      <c t="s" r="C3">
+        <v>0</v>
+      </c>
+      <c t="s" r="D3">
+        <v>7</v>
+      </c>
+      <c t="s" r="E3">
+        <v>5</v>
+      </c>
+      <c t="s" r="F3">
+        <v>1</v>
+      </c>
+      <c t="s" r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row spans="1:7" r="4">
+      <c t="n" r="A4">
+        <v>1.1540000438690186</v>
+      </c>
+      <c t="n" r="B4">
+        <v>568</v>
+      </c>
+      <c t="n" r="C4">
+        <v>0</v>
+      </c>
+      <c t="n" r="D4">
+        <v>550</v>
+      </c>
+      <c t="n" r="E4">
+        <v>400</v>
+      </c>
+      <c t="n" r="F4">
+        <v>1.835051544726403</v>
+      </c>
+      <c t="n" r="G4">
+        <v>-1.2344587604779673</v>
+      </c>
+    </row>
+    <row spans="1:7" r="5">
+      <c t="n" r="A5">
+        <v>41.15299987792969</v>
+      </c>
+      <c t="n" r="B5">
+        <v>585</v>
+      </c>
+      <c t="n" r="C5">
+        <v>0</v>
+      </c>
+      <c t="n" r="D5">
+        <v>550</v>
+      </c>
+      <c t="n" r="E5">
+        <v>1000</v>
+      </c>
+      <c t="n" r="F5">
+        <v>1.9626355897878909</v>
+      </c>
+      <c t="n" r="G5">
+        <v>-1.3243942391810428</v>
+      </c>
+    </row>
+    <row spans="1:7" r="6">
+      <c t="n" r="A6">
+        <v>81.16700005531311</v>
+      </c>
+      <c t="n" r="B6">
+        <v>374</v>
+      </c>
+      <c t="n" r="C6">
+        <v>0</v>
+      </c>
+      <c t="n" r="D6">
+        <v>550</v>
+      </c>
+      <c t="n" r="E6">
+        <v>20</v>
+      </c>
+      <c t="n" r="F6">
+        <v>1.3028082406003572</v>
+      </c>
+      <c t="n" r="G6">
+        <v>-0.3881461001197237</v>
+      </c>
+    </row>
+    <row spans="1:7" r="7">
+      <c t="n" r="A7">
+        <v>121.18099999427795</v>
+      </c>
+      <c t="n" r="B7">
+        <v>363</v>
+      </c>
+      <c t="n" r="C7">
+        <v>0</v>
+      </c>
+      <c t="n" r="D7">
+        <v>550</v>
+      </c>
+      <c t="n" r="E7">
+        <v>1000</v>
+      </c>
+      <c t="n" r="F7">
+        <v>0.9791546236015368</v>
+      </c>
+      <c t="n" r="G7">
+        <v>-0.1600456713471313</v>
+      </c>
+    </row>
+    <row spans="1:7" r="8">
+      <c t="n" r="A8">
+        <v>161.1949999332428</v>
+      </c>
+      <c t="n" r="B8">
+        <v>401</v>
+      </c>
+      <c t="n" r="C8">
+        <v>0</v>
+      </c>
+      <c t="n" r="D8">
+        <v>550</v>
+      </c>
+      <c t="n" r="E8">
+        <v>1000</v>
+      </c>
+      <c t="n" r="F8">
+        <v>0.7844271095341199</v>
+      </c>
+      <c t="n" r="G8">
+        <v>0.11625218531182316</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
     <col min="1" width="9.10" max="1"/>
     <col min="2" width="9.10" max="2"/>
     <col min="3" width="9.10" max="3"/>
@@ -10464,7 +11207,7 @@
         <v>3</v>
       </c>
       <c t="s" r="B1">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row spans="1:7" r="3">
@@ -10492,508 +11235,738 @@
     </row>
     <row spans="1:7" r="4">
       <c t="n" r="A4">
-        <v>0.0009999275207519531</v>
+        <v>1.1389999389648438</v>
       </c>
       <c t="n" r="B4">
-        <v>35.933199283626188</v>
+        <v>589</v>
       </c>
       <c t="n" r="C4">
         <v>0</v>
       </c>
       <c t="n" r="D4">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E4">
-        <v>40</v>
+        <v>678</v>
       </c>
       <c t="n" r="F4">
-        <v>0.87268835927578337</v>
+        <v>0.68686068511482601</v>
       </c>
       <c t="n" r="G4">
-        <v>0.14046549089770402</v>
+        <v>0.32597690486900044</v>
       </c>
     </row>
     <row spans="1:7" r="5">
       <c t="n" r="A5">
-        <v>40.00099992752075</v>
+        <v>41.15300011634827</v>
       </c>
       <c t="n" r="B5">
-        <v>39.033975167287515</v>
+        <v>599</v>
       </c>
       <c t="n" r="C5">
         <v>0</v>
       </c>
       <c t="n" r="D5">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E5">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c t="n" r="F5">
-        <v>0.71635465691739375</v>
+        <v>0.69722272079296277</v>
       </c>
       <c t="n" r="G5">
-        <v>0.33392070384818118</v>
+        <v>0.27715733382544061</v>
       </c>
     </row>
     <row spans="1:7" r="6">
       <c t="n" r="A6">
-        <v>80.0019998550415</v>
+        <v>81.15300011634827</v>
       </c>
       <c t="n" r="B6">
-        <v>31.034834916987968</v>
+        <v>626</v>
       </c>
       <c t="n" r="C6">
         <v>0</v>
       </c>
       <c t="n" r="D6">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E6">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c t="n" r="F6">
-        <v>1.4517732416005811</v>
+        <v>0.53174175655778566</v>
       </c>
       <c t="n" r="G6">
-        <v>-0.25601925712454654</v>
+        <v>0.30909495720171243</v>
       </c>
     </row>
     <row spans="1:7" r="7">
       <c t="n" r="A7">
-        <v>120.00099992752075</v>
+        <v>121.15199995040894</v>
       </c>
       <c t="n" r="B7">
-        <v>22.977419850428806</v>
+        <v>634</v>
       </c>
       <c t="n" r="C7">
         <v>0</v>
       </c>
       <c t="n" r="D7">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E7">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c t="n" r="F7">
-        <v>0.74189163491884103</v>
+        <v>0.53375929801816602</v>
       </c>
       <c t="n" r="G7">
-        <v>0.62980636572869775</v>
+        <v>0.29978024879043058</v>
       </c>
     </row>
     <row spans="1:7" r="8">
       <c t="n" r="A8">
-        <v>160.0</v>
+        <v>161.15100002288818</v>
       </c>
       <c t="n" r="B8">
-        <v>27.706051296647992</v>
+        <v>569</v>
       </c>
       <c t="n" r="C8">
         <v>0</v>
       </c>
       <c t="n" r="D8">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E8">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c t="n" r="F8">
-        <v>1.2043497720614438</v>
+        <v>0.37526607035754761</v>
       </c>
       <c t="n" r="G8">
-        <v>0.25884948477102326</v>
+        <v>0.33251273482580879</v>
       </c>
     </row>
     <row spans="1:7" r="9">
       <c t="n" r="A9">
-        <v>199.99899983406067</v>
+        <v>201.16499996185303</v>
       </c>
       <c t="n" r="B9">
-        <v>30.736924145713509</v>
+        <v>505</v>
       </c>
       <c t="n" r="C9">
         <v>0</v>
       </c>
       <c t="n" r="D9">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E9">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c t="n" r="F9">
-        <v>1.4992702757300553</v>
+        <v>0.093699229929797512</v>
       </c>
       <c t="n" r="G9">
-        <v>-0.1078971777120829</v>
+        <v>1.5370924451067367</v>
       </c>
     </row>
     <row spans="1:7" r="10">
       <c t="n" r="A10">
-        <v>239.99899983406067</v>
+        <v>241.17899990081787</v>
       </c>
       <c t="n" r="B10">
-        <v>22.946814329570003</v>
+        <v>513</v>
       </c>
       <c t="n" r="C10">
         <v>0</v>
       </c>
       <c t="n" r="D10">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E10">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c t="n" r="F10">
-        <v>1.747515042021345</v>
+        <v>0.10366274695932234</v>
       </c>
       <c t="n" r="G10">
-        <v>-0.30757613766259773</v>
+        <v>1.5352141080693247</v>
       </c>
     </row>
     <row spans="1:7" r="11">
       <c t="n" r="A11">
-        <v>279.9979999065399</v>
+        <v>281.1930000782013</v>
       </c>
       <c t="n" r="B11">
-        <v>26.8511666315705</v>
+        <v>535</v>
       </c>
       <c t="n" r="C11">
         <v>0</v>
       </c>
       <c t="n" r="D11">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E11">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c t="n" r="F11">
-        <v>1.1723917286256109</v>
+        <v>0.3370930105484774</v>
       </c>
       <c t="n" r="G11">
-        <v>0.40805590313024753</v>
+        <v>0.34728376900790714</v>
       </c>
     </row>
     <row spans="1:7" r="12">
       <c t="n" r="A12">
-        <v>319.99899983406067</v>
+        <v>321.20700001716614</v>
       </c>
       <c t="n" r="B12">
-        <v>19.213726524474922</v>
+        <v>477</v>
       </c>
       <c t="n" r="C12">
         <v>0</v>
       </c>
       <c t="n" r="D12">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E12">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c t="n" r="F12">
-        <v>2.1593558802490138</v>
+        <v>0.19741544398127248</v>
       </c>
       <c t="n" r="G12">
-        <v>-0.38735145614649802</v>
+        <v>0.37298945925106458</v>
       </c>
     </row>
     <row spans="1:7" r="13">
       <c t="n" r="A13">
-        <v>359.99899983406067</v>
+        <v>361.20700001716614</v>
       </c>
       <c t="n" r="B13">
-        <v>24.686907023340694</v>
+        <v>406</v>
       </c>
       <c t="n" r="C13">
         <v>0</v>
       </c>
       <c t="n" r="D13">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E13">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c t="n" r="F13">
-        <v>1.2896920391939184</v>
+        <v>-0.048012492249622035</v>
       </c>
       <c t="n" r="G13">
-        <v>0.69264124781664871</v>
+        <v>1.4642405367004683</v>
       </c>
     </row>
     <row spans="1:7" r="14">
       <c t="n" r="A14">
-        <v>399.9979999065399</v>
+        <v>401.2079999446869</v>
       </c>
       <c t="n" r="B14">
-        <v>16.980293681050728</v>
+        <v>429</v>
       </c>
       <c t="n" r="C14">
         <v>0</v>
       </c>
       <c t="n" r="D14">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E14">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c t="n" r="F14">
-        <v>2.7879320516502331</v>
+        <v>-0.022675251159384922</v>
       </c>
       <c t="n" r="G14">
-        <v>-0.51797979587155496</v>
+        <v>1.4597573918351239</v>
       </c>
     </row>
     <row spans="1:7" r="15">
       <c t="n" r="A15">
-        <v>439.9979999065399</v>
+        <v>441.20700001716614</v>
       </c>
       <c t="n" r="B15">
-        <v>11.026008525667306</v>
+        <v>444</v>
       </c>
       <c t="n" r="C15">
         <v>0</v>
       </c>
       <c t="n" r="D15">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E15">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c t="n" r="F15">
-        <v>0.66443253229346455</v>
+        <v>0.19226769739330471</v>
       </c>
       <c t="n" r="G15">
-        <v>2.1120972295494149</v>
+        <v>0.34251446024928955</v>
       </c>
     </row>
     <row spans="1:7" r="16">
       <c t="n" r="A16">
-        <v>479.9979999065399</v>
+        <v>481.20700001716614</v>
       </c>
       <c t="n" r="B16">
-        <v>6.2319110066307131</v>
+        <v>403</v>
       </c>
       <c t="n" r="C16">
         <v>0</v>
       </c>
       <c t="n" r="D16">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E16">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c t="n" r="F16">
-        <v>0.56653503371161673</v>
+        <v>0.10469799047697848</v>
       </c>
       <c t="n" r="G16">
-        <v>2.1913795671040268</v>
+        <v>0.35789129566605832</v>
       </c>
     </row>
     <row spans="1:7" r="17">
       <c t="n" r="A17">
-        <v>519.9979999065399</v>
+        <v>521.220999956131</v>
       </c>
       <c t="n" r="B17">
-        <v>13.35249149398372</v>
+        <v>338</v>
       </c>
       <c t="n" r="C17">
         <v>0</v>
       </c>
       <c t="n" r="D17">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E17">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c t="n" r="F17">
-        <v>2.0639738616114385</v>
+        <v>-0.13894523787685956</v>
       </c>
       <c t="n" r="G17">
-        <v>0.35287833189541828</v>
+        <v>1.3522551289996447</v>
       </c>
     </row>
     <row spans="1:7" r="18">
       <c t="n" r="A18">
-        <v>559.9979999065399</v>
+        <v>561.2350001335144</v>
       </c>
       <c t="n" r="B18">
-        <v>19.057098349076064</v>
+        <v>289</v>
       </c>
       <c t="n" r="C18">
         <v>0</v>
       </c>
       <c t="n" r="D18">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E18">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c t="n" r="F18">
-        <v>2.6906336488950298</v>
+        <v>-0.37502489952609641</v>
       </c>
       <c t="n" r="G18">
-        <v>-0.16853125826269044</v>
+        <v>1.3967556667027474</v>
       </c>
     </row>
     <row spans="1:7" r="19">
       <c t="n" r="A19">
-        <v>599.9969999790192</v>
+        <v>601.2490000724792</v>
       </c>
       <c t="n" r="B19">
-        <v>13.443004177115851</v>
+        <v>298</v>
       </c>
       <c t="n" r="C19">
         <v>0</v>
       </c>
       <c t="n" r="D19">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E19">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c t="n" r="F19">
-        <v>2.8980685583962682</v>
+        <v>-0.36121439827399021</v>
       </c>
       <c t="n" r="G19">
-        <v>-0.41778593517381774</v>
+        <v>1.33787475018741</v>
       </c>
     </row>
     <row spans="1:7" r="20">
       <c t="n" r="A20">
-        <v>639.9979999065399</v>
+        <v>641.2630000114441</v>
       </c>
       <c t="n" r="B20">
-        <v>8.1476934726120582</v>
+        <v>338</v>
       </c>
       <c t="n" r="C20">
         <v>0</v>
       </c>
       <c t="n" r="D20">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E20">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c t="n" r="F20">
-        <v>0.62716062044722198</v>
+        <v>-4.5826567227576414</v>
       </c>
       <c t="n" r="G20">
-        <v>1.4708368390401685</v>
+        <v>1.8643837993413785</v>
       </c>
     </row>
     <row spans="1:7" r="21">
       <c t="n" r="A21">
-        <v>679.9979999065399</v>
+        <v>681.2769999504089</v>
       </c>
       <c t="n" r="B21">
-        <v>4.0294211788104368</v>
+        <v>379</v>
       </c>
       <c t="n" r="C21">
         <v>0</v>
       </c>
       <c t="n" r="D21">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E21">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c t="n" r="F21">
-        <v>0.49844895905867143</v>
+        <v>-4.6085351685365401</v>
       </c>
       <c t="n" r="G21">
-        <v>1.625075160969069</v>
+        <v>1.939083991261612</v>
       </c>
     </row>
     <row spans="1:7" r="22">
       <c t="n" r="A22">
-        <v>719.9979999065399</v>
+        <v>721.2760000228882</v>
       </c>
       <c t="n" r="B22">
-        <v>1.1388019894559074</v>
+        <v>330</v>
       </c>
       <c t="n" r="C22">
         <v>0</v>
       </c>
       <c t="n" r="D22">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E22">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c t="n" r="F22">
-        <v>0.3029409353122563</v>
+        <v>-2.9464118568400752</v>
       </c>
       <c t="n" r="G22">
-        <v>1.7899812102016348</v>
+        <v>1.4065093593687608</v>
       </c>
     </row>
     <row spans="1:7" r="23">
       <c t="n" r="A23">
-        <v>759.9969999790192</v>
+        <v>761.289999961853</v>
       </c>
       <c t="n" r="B23">
-        <v>10.271096523958475</v>
+        <v>356</v>
       </c>
       <c t="n" r="C23">
         <v>0</v>
       </c>
       <c t="n" r="D23">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E23">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c t="n" r="F23">
-        <v>3.7670957387779218</v>
+        <v>-12.456212548774667</v>
       </c>
       <c t="n" r="G23">
-        <v>-2.1870212125393547</v>
+        <v>15.846030379043878</v>
       </c>
     </row>
     <row spans="1:7" r="24">
       <c t="n" r="A24">
-        <v>799.9979999065399</v>
+        <v>801.3039999008179</v>
       </c>
       <c t="n" r="B24">
-        <v>5.6107300908496764</v>
+        <v>307</v>
       </c>
       <c t="n" r="C24">
         <v>0</v>
       </c>
       <c t="n" r="D24">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E24">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c t="n" r="F24">
-        <v>1.7628509569017332</v>
+        <v>108.20552763006091</v>
       </c>
       <c t="n" r="G24">
-        <v>-0.12551221072150787</v>
+        <v>-41.971805818191243</v>
       </c>
     </row>
     <row spans="1:7" r="25">
       <c t="n" r="A25">
-        <v>839.9979999065399</v>
+        <v>841.3499999046326</v>
       </c>
       <c t="n" r="B25">
-        <v>2.1973201275748835</v>
+        <v>329</v>
       </c>
       <c t="n" r="C25">
         <v>0</v>
       </c>
       <c t="n" r="D25">
-        <v>40.0</v>
+        <v>550</v>
       </c>
       <c t="n" r="E25">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c t="n" r="F25">
-        <v>0.46599514819084353</v>
+        <v>136.78306291413497</v>
       </c>
       <c t="n" r="G25">
-        <v>1.1352072927234342</v>
+        <v>-144.61447557053083</v>
+      </c>
+    </row>
+    <row spans="1:7" r="26">
+      <c t="n" r="A26">
+        <v>881.3129999637604</v>
+      </c>
+      <c t="n" r="B26">
+        <v>289</v>
+      </c>
+      <c t="n" r="C26">
+        <v>0</v>
+      </c>
+      <c t="n" r="D26">
+        <v>550</v>
+      </c>
+      <c t="n" r="E26">
+        <v>300</v>
+      </c>
+      <c t="n" r="F26">
+        <v>686.98381228861103</v>
+      </c>
+      <c t="n" r="G26">
+        <v>-242.2828861874147</v>
+      </c>
+    </row>
+    <row spans="1:7" r="27">
+      <c t="n" r="A27">
+        <v>921.3269999027252</v>
+      </c>
+      <c t="n" r="B27">
+        <v>310</v>
+      </c>
+      <c t="n" r="C27">
+        <v>0</v>
+      </c>
+      <c t="n" r="D27">
+        <v>550</v>
+      </c>
+      <c t="n" r="E27">
+        <v>1000</v>
+      </c>
+      <c t="n" r="F27">
+        <v>975.54786765645315</v>
+      </c>
+      <c t="n" r="G27">
+        <v>-987.50231429005316</v>
+      </c>
+    </row>
+    <row spans="1:7" r="28">
+      <c t="n" r="A28">
+        <v>961.3410000801086</v>
+      </c>
+      <c t="n" r="B28">
+        <v>270</v>
+      </c>
+      <c t="n" r="C28">
+        <v>0</v>
+      </c>
+      <c t="n" r="D28">
+        <v>550</v>
+      </c>
+      <c t="n" r="E28">
+        <v>300</v>
+      </c>
+      <c t="n" r="F28">
+        <v>9120.9208178755089</v>
+      </c>
+      <c t="n" r="G28">
+        <v>-3136.8101219899431</v>
+      </c>
+    </row>
+    <row spans="1:7" r="29">
+      <c t="n" r="A29">
+        <v>1001.3399999141693</v>
+      </c>
+      <c t="n" r="B29">
+        <v>218</v>
+      </c>
+      <c t="n" r="C29">
+        <v>0</v>
+      </c>
+      <c t="n" r="D29">
+        <v>550</v>
+      </c>
+      <c t="n" r="E29">
+        <v>300</v>
+      </c>
+      <c t="n" r="F29">
+        <v>58592.981270773016</v>
+      </c>
+      <c t="n" r="G29">
+        <v>-58106.2444840678</v>
+      </c>
+    </row>
+    <row spans="1:7" r="30">
+      <c t="n" r="A30">
+        <v>1041.3399999141693</v>
+      </c>
+      <c t="n" r="B30">
+        <v>246</v>
+      </c>
+      <c t="n" r="C30">
+        <v>0</v>
+      </c>
+      <c t="n" r="D30">
+        <v>550</v>
+      </c>
+      <c t="n" r="E30">
+        <v>1000</v>
+      </c>
+      <c t="n" r="F30">
+        <v>180622.1689966738</v>
+      </c>
+      <c t="n" r="G30">
+        <v>-145595.9848855123</v>
+      </c>
+    </row>
+    <row spans="1:7" r="31">
+      <c t="n" r="A31">
+        <v>1081.3420000076294</v>
+      </c>
+      <c t="n" r="B31">
+        <v>204</v>
+      </c>
+      <c t="n" r="C31">
+        <v>0</v>
+      </c>
+      <c t="n" r="D31">
+        <v>550</v>
+      </c>
+      <c t="n" r="E31">
+        <v>300</v>
+      </c>
+      <c t="n" r="F31">
+        <v>-114588.92578631671</v>
+      </c>
+      <c t="n" r="G31">
+        <v>65913.868328501499</v>
+      </c>
+    </row>
+    <row spans="1:7" r="32">
+      <c t="n" r="A32">
+        <v>1121.3420000076294</v>
+      </c>
+      <c t="n" r="B32">
+        <v>162</v>
+      </c>
+      <c t="n" r="C32">
+        <v>0</v>
+      </c>
+      <c t="n" r="D32">
+        <v>550</v>
+      </c>
+      <c t="n" r="E32">
+        <v>300</v>
+      </c>
+      <c t="n" r="F32">
+        <v>-130231.90864242007</v>
+      </c>
+      <c t="n" r="G32">
+        <v>91669.682861291134</v>
+      </c>
+    </row>
+    <row spans="1:7" r="33">
+      <c t="n" r="A33">
+        <v>1161.3559999465942</v>
+      </c>
+      <c t="n" r="B33">
+        <v>117</v>
+      </c>
+      <c t="n" r="C33">
+        <v>0</v>
+      </c>
+      <c t="n" r="D33">
+        <v>550</v>
+      </c>
+      <c t="n" r="E33">
+        <v>300</v>
+      </c>
+      <c t="n" r="F33">
+        <v>-219586.82034631429</v>
+      </c>
+      <c t="n" r="G33">
+        <v>132412.69483313532</v>
+      </c>
+    </row>
+    <row spans="1:7" r="34">
+      <c t="n" r="A34">
+        <v>1201.3700001239777</v>
+      </c>
+      <c t="n" r="B34">
+        <v>155</v>
+      </c>
+      <c t="n" r="C34">
+        <v>0</v>
+      </c>
+      <c t="n" r="D34">
+        <v>550</v>
+      </c>
+      <c t="n" r="E34">
+        <v>1000</v>
+      </c>
+      <c t="n" r="F34">
+        <v>524533.24834138737</v>
+      </c>
+      <c t="n" r="G34">
+        <v>-460603.64760440914</v>
+      </c>
+    </row>
+    <row spans="1:7" r="35">
+      <c t="n" r="A35">
+        <v>1241.3840000629425</v>
+      </c>
+      <c t="n" r="B35">
+        <v>195</v>
+      </c>
+      <c t="n" r="C35">
+        <v>0</v>
+      </c>
+      <c t="n" r="D35">
+        <v>550</v>
+      </c>
+      <c t="n" r="E35">
+        <v>1000</v>
+      </c>
+      <c t="n" r="F35">
+        <v>533563.49615443428</v>
+      </c>
+      <c t="n" r="G35">
+        <v>-106123.08078996232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>